<commit_message>
Update USAW age groups and BARS results
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/USAW-BARSResults.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/USAW-BARSResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\protocol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/usaw-owlcms/local/templates/competitionResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4556591-0842-45B0-8A61-0C3ECAE3E3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D688D01-3CD4-5E4C-A145-AB34EAA840FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2805" windowWidth="21600" windowHeight="11295" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="33480" yWindow="1560" windowWidth="38540" windowHeight="21200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Scott Gonzalez</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{12B6AA44-0487-684F-B036-44816B8A7B93}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:area(lastCell="L2")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5FDBE4AB-8743-D745-B118-5469DFB1B5E3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">jx:each(
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  items="athletes"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  var="athlete"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  lastCell="L2"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
   <si>
     <t>Lifter Membership ID</t>
   </si>
@@ -64,45 +140,9 @@
     <t>Clean &amp; Jerk Weight (kg) 3</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${lifters}" var="l" varStatus="lifterLoop"&gt;</t>
-  </si>
-  <si>
-    <t>${l.membership}</t>
-  </si>
-  <si>
     <t>${competition.competitionDate}</t>
   </si>
   <si>
-    <t>$[VLOOKUP(L3, Validation!$C$1:$D$29,2,FALSE)]</t>
-  </si>
-  <si>
-    <t>${l.bodyWeight}</t>
-  </si>
-  <si>
-    <t>${l.snatch1AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.snatch2AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.snatch3AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.cleanJerk1AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.cleanJerk2AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.cleanJerk3AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.ageGroup}</t>
-  </si>
-  <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
-  <si>
     <t>Men's 16-17 Age Group</t>
   </si>
   <si>
@@ -281,17 +321,98 @@
   </si>
   <si>
     <t>M80</t>
+  </si>
+  <si>
+    <t>W80</t>
+  </si>
+  <si>
+    <t>M85</t>
+  </si>
+  <si>
+    <t>W85</t>
+  </si>
+  <si>
+    <t>M90</t>
+  </si>
+  <si>
+    <t>W90</t>
+  </si>
+  <si>
+    <t>M95</t>
+  </si>
+  <si>
+    <t>W95</t>
+  </si>
+  <si>
+    <t>M100</t>
+  </si>
+  <si>
+    <t>W100</t>
+  </si>
+  <si>
+    <t>U25 M</t>
+  </si>
+  <si>
+    <t>U25 F</t>
+  </si>
+  <si>
+    <t>U23 M</t>
+  </si>
+  <si>
+    <t>U23 F</t>
+  </si>
+  <si>
+    <t>U11 M</t>
+  </si>
+  <si>
+    <t>U11 F</t>
+  </si>
+  <si>
+    <t>ADP M</t>
+  </si>
+  <si>
+    <t>ADP F</t>
+  </si>
+  <si>
+    <t>$[VLOOKUP(L2, Validation!$A$1:$B$48,2,FALSE)]</t>
+  </si>
+  <si>
+    <t>${athlete.membership}</t>
+  </si>
+  <si>
+    <t>${athlete.bodyWeight}</t>
+  </si>
+  <si>
+    <t>${athlete.snatch1AsInteger}</t>
+  </si>
+  <si>
+    <t>${athlete.snatch2AsInteger}</t>
+  </si>
+  <si>
+    <t>${athlete.snatch3AsInteger}</t>
+  </si>
+  <si>
+    <t>${athlete.cleanJerk1AsInteger}</t>
+  </si>
+  <si>
+    <t>${athlete.cleanJerk2AsInteger}</t>
+  </si>
+  <si>
+    <t>${athlete.cleanJerk3AsInteger}</t>
+  </si>
+  <si>
+    <t>${athlete.ageGroup}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0;\(0\);\-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -316,6 +437,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -337,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -347,43 +480,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -400,10 +510,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2025650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4648200" cy="1752600"/>
     <xdr:sp macro="" textlink="" fLocksText="0">
@@ -421,7 +531,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4591050" y="1552575"/>
+          <a:off x="4044950" y="1206500"/>
           <a:ext cx="4648200" cy="1752600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -993,25 +1103,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
     <col min="4" max="4" width="22" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.625" customWidth="1"/>
-    <col min="6" max="7" width="30.125" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="7" width="30.1640625" customWidth="1"/>
     <col min="8" max="10" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21.75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="23" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1044,477 +1152,468 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2"/>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4"/>
-      <c r="D4"/>
-      <c r="J4" s="16"/>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <conditionalFormatting sqref="D4:F4">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>AND((C3),C3,C3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="date" allowBlank="1" showErrorMessage="1" sqref="B1 B5:B1004">
+  <dataValidations count="4">
+    <dataValidation type="date" allowBlank="1" showErrorMessage="1" sqref="B1 B3:B1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
       <formula2>54789</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="A3 A5:A1004">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="A3:A1002" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="D1 D3 D5:D1004">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="D1 D3:D1002" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>20</formula1>
       <formula2>300</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="E1:J1 E5:J1004">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="E1:J1 E3:J1002" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>-500</formula1>
       <formula2>500</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="H4">
-      <formula1>0</formula1>
-      <formula2>200</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView zoomScale="163" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="26.25" customWidth="1"/>
+    <col min="2" max="3" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="str">
-        <f t="shared" ref="D1:D31" si="0">A1</f>
-        <v>Men's 16-17 Age Group</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's 16-17 Age Group</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's 14-15 Age Group</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's 14-15 Age Group</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's 13 Under Age Group</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's 13 Under Age Group</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>Junior Men's</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>Junior Women's</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>Open Men's</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>Open Women's</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>Open Men's</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>Open Women's</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (35-39)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (35-39)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (40-44)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (40-44)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (45-49)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (45-49)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
         <v>57</v>
       </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (50-54)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (50-54)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (55-59)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (55-59)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
         <v>65</v>
       </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (60-64)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (60-64)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
         <v>69</v>
       </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (65-69)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (65-69)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>73</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>74</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (70-74)</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>75</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>76</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (70-74)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>77</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (75-79)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B47" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>Women's Masters (75+)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>Men's Masters (80+)</v>
-      </c>
+      <c r="B48" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="E48" s="11"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>